<commit_message>
add to example omop spreadsheets
</commit_message>
<xml_diff>
--- a/examples/omop/omop-schemas.xlsx
+++ b/examples/omop/omop-schemas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="76">
   <si>
     <t>https://lschema.org/valueType</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Schema</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>Object</t>
@@ -299,13 +302,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -642,19 +642,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="43.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="33.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="34.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="43.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="34.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="8"/>
+      <c r="B1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
@@ -663,237 +663,237 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="7" t="s">
-        <v>57</v>
+      <c r="A3" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9">
-        <f>TRUE()</f>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="7" t="s">
-        <v>56</v>
+      <c r="A4" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="C4" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="10" t="s">
         <v>9</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -912,17 +912,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="53.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="46.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="55.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="53.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="46.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="55.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>48</v>
+      <c r="B1" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="C1" s="2"/>
     </row>
@@ -939,88 +939,88 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <f>TRUE()</f>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="7" t="s">
-        <v>48</v>
+      <c r="A4" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
@@ -1989,9 +1989,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="52.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="47.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="52.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="47.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="34.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1999,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2"/>
     </row>
@@ -2016,132 +2016,132 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <f>TRUE()</f>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
@@ -2175,8 +2175,8 @@
       <c r="C20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="6" t="s">
-        <v>47</v>
+      <c r="A21" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3092,9 +3092,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="41.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="52.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="66.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="41.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="52.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="66.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -3102,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2"/>
     </row>
@@ -3113,72 +3113,72 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <f>TRUE()</f>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
@@ -4157,9 +4157,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="62.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="51.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="30.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="62.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="51.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="30.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -4167,7 +4167,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2"/>
     </row>
@@ -4184,99 +4184,99 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <f>TRUE()</f>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
@@ -5240,9 +5240,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="50.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="50.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="47.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="50.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="50.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="47.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -5272,8 +5272,8 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <f>TRUE()</f>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
@@ -5281,118 +5281,118 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">

</xml_diff>